<commit_message>
Bulkupload units reset and cancel redirecting to manual units new ui
</commit_message>
<xml_diff>
--- a/src/assets/Excel/Demo_Unit_Detailstemplate_New.xlsx
+++ b/src/assets/Excel/Demo_Unit_Detailstemplate_New.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\oyespace6-5-2020\18-05-2020\OyeSocietyWeb\src\assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anusha\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055ADFED-A46B-4F9D-B38B-7AB35BDCA695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{175161DC-EDBA-4FF4-BC89-69CAF931EF3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Sno</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>UnSold Tenant Occupied Unit</t>
+  </si>
+  <si>
+    <t>VILLA</t>
   </si>
 </sst>
 </file>
@@ -1580,14 +1583,14 @@
   <dimension ref="A1:IV6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="15.15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
@@ -1888,7 +1891,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>33</v>
@@ -3238,9 +3241,12 @@
       <c r="IT6" s="19"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{B6B10155-E097-4F97-B54D-F946A9243B59}">
       <formula1>"Sold Owner Occupied Unit,Sold Tenant Occupied Unit,Sold Vacant Unit,UnSold Vacant Unit,UnSold Tenant Occupied Unit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{1B2E9E41-DB47-4BCC-867F-E5A8CA67F5C6}">
+      <formula1>"FLAT,VILLA,VACCANT PLOT"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>